<commit_message>
excel del 8 de noviembre
</commit_message>
<xml_diff>
--- a/m1/unidad3/Practicas/20191107/EjExcAva-Pra2.xlsx
+++ b/m1/unidad3/Practicas/20191107/EjExcAva-Pra2.xlsx
@@ -215,7 +215,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -299,8 +299,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -610,7 +610,7 @@
   <dimension ref="A1:AG38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -627,7 +627,9 @@
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="18" width="12.140625" customWidth="1"/>
+    <col min="15" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
     <col min="19" max="19" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -773,8 +775,8 @@
         <v>0</v>
       </c>
       <c r="Q4" s="10">
-        <f ca="1">(YEAR(TODAY())-YEAR(C4))</f>
-        <v>63</v>
+        <f ca="1">YEARFRAC(C4,TODAY())</f>
+        <v>63.244444444444447</v>
       </c>
       <c r="R4" s="14">
         <f>IF(O4&lt;5000,300,IF(AND(O4&gt;=5000,O4&lt;=10000),IF(E4="Jornalero",200,100),"N/A"))</f>
@@ -836,8 +838,8 @@
         <v>200</v>
       </c>
       <c r="Q5" s="10">
-        <f t="shared" ref="Q5:Q32" ca="1" si="8">(YEAR(TODAY())-YEAR(C5))</f>
-        <v>58</v>
+        <f t="shared" ref="Q5:Q32" ca="1" si="8">YEARFRAC(C5,TODAY())</f>
+        <v>58.580555555555556</v>
       </c>
       <c r="R5" s="14">
         <f t="shared" ref="R5:R32" si="9">IF(O5&lt;5000,300,IF(AND(O5&gt;=5000,O5&lt;=10000),IF(E5="Jornalero",200,100),"N/A"))</f>
@@ -900,7 +902,7 @@
       </c>
       <c r="Q6" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>40</v>
+        <v>40.427777777777777</v>
       </c>
       <c r="R6" s="14">
         <f t="shared" si="9"/>
@@ -963,7 +965,7 @@
       </c>
       <c r="Q7" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>54</v>
+        <v>54.31666666666667</v>
       </c>
       <c r="R7" s="14">
         <f t="shared" si="9"/>
@@ -1026,7 +1028,7 @@
       </c>
       <c r="Q8" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>53</v>
+        <v>52.880555555555553</v>
       </c>
       <c r="R8" s="14" t="str">
         <f t="shared" si="9"/>
@@ -1089,7 +1091,7 @@
       </c>
       <c r="Q9" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>37</v>
+        <v>37.241666666666667</v>
       </c>
       <c r="R9" s="14">
         <f t="shared" si="9"/>
@@ -1152,7 +1154,7 @@
       </c>
       <c r="Q10" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>45</v>
+        <v>45.086111111111109</v>
       </c>
       <c r="R10" s="14">
         <f t="shared" si="9"/>
@@ -1215,7 +1217,7 @@
       </c>
       <c r="Q11" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>41</v>
+        <v>41.272222222222226</v>
       </c>
       <c r="R11" s="14">
         <f t="shared" si="9"/>
@@ -1278,7 +1280,7 @@
       </c>
       <c r="Q12" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>60</v>
+        <v>60.508333333333333</v>
       </c>
       <c r="R12" s="14">
         <f t="shared" si="9"/>
@@ -1341,7 +1343,7 @@
       </c>
       <c r="Q13" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>49</v>
+        <v>49.138888888888886</v>
       </c>
       <c r="R13" s="14">
         <f t="shared" si="9"/>
@@ -1404,7 +1406,7 @@
       </c>
       <c r="Q14" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>43</v>
+        <v>43.236111111111114</v>
       </c>
       <c r="R14" s="14">
         <f t="shared" si="9"/>
@@ -1467,7 +1469,7 @@
       </c>
       <c r="Q15" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>57</v>
+        <v>56.916666666666664</v>
       </c>
       <c r="R15" s="14">
         <f t="shared" si="9"/>
@@ -1530,7 +1532,7 @@
       </c>
       <c r="Q16" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>50</v>
+        <v>50.302777777777777</v>
       </c>
       <c r="R16" s="14">
         <f t="shared" si="9"/>
@@ -1593,7 +1595,7 @@
       </c>
       <c r="Q17" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>70</v>
+        <v>70.25833333333334</v>
       </c>
       <c r="R17" s="14">
         <f t="shared" si="9"/>
@@ -1656,7 +1658,7 @@
       </c>
       <c r="Q18" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>60</v>
+        <v>60.783333333333331</v>
       </c>
       <c r="R18" s="14" t="str">
         <f t="shared" si="9"/>
@@ -1719,7 +1721,7 @@
       </c>
       <c r="Q19" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>50</v>
+        <v>50.68888888888889</v>
       </c>
       <c r="R19" s="14">
         <f t="shared" si="9"/>
@@ -1782,7 +1784,7 @@
       </c>
       <c r="Q20" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>42</v>
+        <v>42.8</v>
       </c>
       <c r="R20" s="14">
         <f t="shared" si="9"/>
@@ -1845,7 +1847,7 @@
       </c>
       <c r="Q21" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>51</v>
+        <v>51.174999999999997</v>
       </c>
       <c r="R21" s="14">
         <f t="shared" si="9"/>
@@ -1908,7 +1910,7 @@
       </c>
       <c r="Q22" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>46</v>
+        <v>46.49722222222222</v>
       </c>
       <c r="R22" s="14">
         <f t="shared" si="9"/>
@@ -1971,7 +1973,7 @@
       </c>
       <c r="Q23" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>39</v>
+        <v>39.180555555555557</v>
       </c>
       <c r="R23" s="14">
         <f t="shared" si="9"/>
@@ -2034,7 +2036,7 @@
       </c>
       <c r="Q24" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>51</v>
+        <v>50.994444444444447</v>
       </c>
       <c r="R24" s="14">
         <f t="shared" si="9"/>
@@ -2097,7 +2099,7 @@
       </c>
       <c r="Q25" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>59</v>
+        <v>59.255555555555553</v>
       </c>
       <c r="R25" s="14">
         <f t="shared" si="9"/>
@@ -2160,7 +2162,7 @@
       </c>
       <c r="Q26" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>41</v>
+        <v>40.863888888888887</v>
       </c>
       <c r="R26" s="14">
         <f t="shared" si="9"/>
@@ -2223,7 +2225,7 @@
       </c>
       <c r="Q27" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>37</v>
+        <v>37.838888888888889</v>
       </c>
       <c r="R27" s="14">
         <f t="shared" si="9"/>
@@ -2286,7 +2288,7 @@
       </c>
       <c r="Q28" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>43</v>
+        <v>43.427777777777777</v>
       </c>
       <c r="R28" s="14">
         <f t="shared" si="9"/>
@@ -2349,7 +2351,7 @@
       </c>
       <c r="Q29" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>50</v>
+        <v>50.452777777777776</v>
       </c>
       <c r="R29" s="14">
         <f t="shared" si="9"/>
@@ -2412,7 +2414,7 @@
       </c>
       <c r="Q30" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>44</v>
+        <v>44.555555555555557</v>
       </c>
       <c r="R30" s="14">
         <f t="shared" si="9"/>
@@ -2475,7 +2477,7 @@
       </c>
       <c r="Q31" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>38</v>
+        <v>37.855555555555554</v>
       </c>
       <c r="R31" s="14">
         <f t="shared" si="9"/>
@@ -2538,7 +2540,7 @@
       </c>
       <c r="Q32" s="10">
         <f t="shared" ca="1" si="8"/>
-        <v>74</v>
+        <v>74.561111111111117</v>
       </c>
       <c r="R32" s="14">
         <f t="shared" si="9"/>

</xml_diff>